<commit_message>
update with data of 08 08 2024
</commit_message>
<xml_diff>
--- a/data/data_excel_to_parquet/cercles.xlsx
+++ b/data/data_excel_to_parquet/cercles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\mbarek\script_python\projet_streamlit\data\data_excel_to_parquet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B03EBF7-E13A-4474-AEA0-5FDE4E36B077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5F1BC4-49A5-4772-A5A4-C1E1CBDB1FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{709A7EC8-ED76-4FB2-B897-AECC28259EE9}"/>
   </bookViews>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:D180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>